<commit_message>
fluxo captcha e salvar status
</commit_message>
<xml_diff>
--- a/Cópia de PROCESSOS TRT2 - FÍSICOS(233).xlsx
+++ b/Cópia de PROCESSOS TRT2 - FÍSICOS(233).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torre\OneDrive\Documentos\UiPath\robô trt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B3BA84-21A0-4D4A-BE48-E38C8F778E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F29E2-4883-4AD3-8413-46CCDE2B5DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4965" yWindow="2790" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processos TRT 2 - Físico" sheetId="1" r:id="rId1"/>
@@ -30,22 +30,22 @@
     <t>Número do Processo</t>
   </si>
   <si>
+    <t>0001880-70.2013.5.02.0202</t>
+  </si>
+  <si>
+    <t>1002201-07.2017.5.02.0604</t>
+  </si>
+  <si>
+    <t>1002201-43.2016.5.02.0086</t>
+  </si>
+  <si>
+    <t>1000728-47.2018.5.02.0055</t>
+  </si>
+  <si>
+    <t>1001068-29.2016.5.02.0065</t>
+  </si>
+  <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>0001880-70.2013.5.02.0202</t>
-  </si>
-  <si>
-    <t>1002201-07.2017.5.02.0604</t>
-  </si>
-  <si>
-    <t>1002201-43.2016.5.02.0086</t>
-  </si>
-  <si>
-    <t>1000728-47.2018.5.02.0055</t>
-  </si>
-  <si>
-    <t>1001068-29.2016.5.02.0065</t>
   </si>
 </sst>
 </file>
@@ -435,36 +435,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>

</xml_diff>

<commit_message>
sequencia de tratamento de erros
</commit_message>
<xml_diff>
--- a/Cópia de PROCESSOS TRT2 - FÍSICOS(233).xlsx
+++ b/Cópia de PROCESSOS TRT2 - FÍSICOS(233).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torre\OneDrive\Documentos\UiPath\robô trt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6CEC54-F086-4563-B2BB-E53B100C7C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BA2A87-4D22-4A29-82F6-A2315747916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4965" yWindow="2790" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
correção de bugs e projeto finalizado
</commit_message>
<xml_diff>
--- a/Cópia de PROCESSOS TRT2 - FÍSICOS(233).xlsx
+++ b/Cópia de PROCESSOS TRT2 - FÍSICOS(233).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torre\OneDrive\Documentos\UiPath\robô trt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BA2A87-4D22-4A29-82F6-A2315747916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A44016-2E39-4743-851A-A214DF391FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4965" yWindow="2790" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>